<commit_message>
Update SD Card BOM
</commit_message>
<xml_diff>
--- a/notes/AVIELF2SD/AVIELF2SD-BOM.xlsx
+++ b/notes/AVIELF2SD/AVIELF2SD-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/AVIELF2SD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{24145382-7CE3-FC47-90D6-8D15D468A74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366272CB-C218-0645-8A5D-BE3550881897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24780" yWindow="2460" windowWidth="31180" windowHeight="19820"/>
+    <workbookView xWindow="26040" yWindow="4240" windowWidth="31180" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIGIKEY.CA" sheetId="1" r:id="rId1"/>
+    <sheet name="DIGIKEY.COM" sheetId="2" r:id="rId2"/>
+    <sheet name="MOUSER.CA" sheetId="3" r:id="rId3"/>
+    <sheet name="MOUSER.COM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="238">
   <si>
     <t>C1, C2</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>C3, C4, C5, C6, C7, C8, C9, C10, C13, C14</t>
   </si>
   <si>
@@ -74,42 +74,9 @@
     <t>J2</t>
   </si>
   <si>
-    <t>Conn_01x06_Socket</t>
-  </si>
-  <si>
-    <t>Connector:Conn_01x06_Socket</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
-    <t xml:space="preserve"> ~</t>
-  </si>
-  <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>Jumper:Jumper_3_Bridged12</t>
-  </si>
-  <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>Jumper:Jumper_2_Bridged</t>
-  </si>
-  <si>
-    <t>JP4, JP5</t>
-  </si>
-  <si>
-    <t>Jumper_2_Open</t>
-  </si>
-  <si>
-    <t>Jumper:Jumper_2_Open</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -401,12 +368,6 @@
     <t>https://www.digikey.ca/en/products/detail/kemet/C320C104K5R5TA7317/6562447</t>
   </si>
   <si>
-    <t>1.0uf Electrolytic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/860020672005/5727088 </t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/vishay-beyschlag-draloric-bc-components/A104K15X7RF5TAA/146011</t>
   </si>
   <si>
@@ -419,9 +380,6 @@
     <t xml:space="preserve">10 kilohm Carbon Film Resistor  </t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT10K0/1741265 </t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT2K00/1741368</t>
   </si>
   <si>
@@ -465,12 +423,339 @@
   </si>
   <si>
     <t>Single 8-Channel Analog Multiplexer or Demultiplexer with Logic-Level Conversion</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>SD CARD ENABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOT (OFF/ON) </t>
+  </si>
+  <si>
+    <t>Alternatively use mini SPDT slide switch: https://www.amazon.ca/dp/B00O9YOEDC</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-pin headers for COM 1 serial </t>
+  </si>
+  <si>
+    <t>JP3, JP4, JP5</t>
+  </si>
+  <si>
+    <t>6-Pin header for TTL/USB Serial Connection</t>
+  </si>
+  <si>
+    <t>Alternatively, use a female 6 pin inline socket</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PREC040SAAN-RC/2774814</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/assmann-wsw-components/A-DF-09-A-KG-T2S/1241800</t>
+  </si>
+  <si>
+    <t>9 Position D-Sub Receptacle, Female Sockets Connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/L78L33ABZ-AP/1663442</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/MAX232N/277048</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD4051BE/67305</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74HC00N/277209</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/toshiba-semiconductor-and-storage/TC74HC04APF/870457</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74HC27N/476055</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HC30E/376837</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HC32E/475930</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74HC74N/277248</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HC157E/1506689</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HC238E/1506865</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74LS259BN/563027</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HC299E/376835</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HC390E/376757</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74HC573AN/277242</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/1N914/978749</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/led-indication-discrete/105</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ECA-1EM100B/2688676</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/C320C104K5R5TA7317/6562447</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-beyschlag-draloric-bc-components/A104K15X7RF5TAA/146011</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT4K70/1741428</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT2K00/1741368</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT1K00/1741314</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT22K0/1741350</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/4609X-101-331LF/3593666</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-cs-fci/10067847-001RLF/2283478</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PREC040SAAN-RC/2774814</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/assmann-wsw-components/A-DF-09-A-KG-T2S/1241800</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT10K0/1741265</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT10K0/1741265</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/STMicroelectronics/L78L33ABZ-AP?qs=7IaIRco65plqHZGvVBuyKw%3D%3D</t>
+  </si>
+  <si>
+    <t>MOUSER</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/MAX232N?qs=5BZzbFV4k2vm92DEZa5XUA%3D%3D</t>
+  </si>
+  <si>
+    <t>Not available at Mouser in UV errasable format. Recommend Jameco: https://www.jameco.com/z/MX27C256DC-15-Macronix-IC-27C256-15-EPROM-256K-Bit-150ns-CMOS-UV-Erasable-Prommable-ROM_39714.html</t>
+  </si>
+  <si>
+    <t>Memory RAM: 628128 DIP32</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD4051BE?qs=q2XTDbzbm6DxulBsMcV7tA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC00E?qs=UGVLDq%2F29ujRl31yA9SdhQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/SN74HC04N?qs=L5CvrNUdZirrSGYiJvTylA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/SN74HC27N?qs=sGAEpiMZZMv4BkFy%252BbL2aPi%252BL8sNTlmrokzu%2FObU0qc%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC30E?qs=tJ5HNKWh3OVq%2F4Pt68gHgg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC32E?qs=tJ5HNKWh3OWln99ctEO0hw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/SN74HC74N?qs=p6YqzpSxLIzMm7Vo1aTZ0w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC157E?qs=YxwvVplHM%2Fl8uv0E9i2LyA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC238E?qs=xFfolx0DHx2djOhmdGyl2g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/SN74LS259BN?qs=SL3LIuy2dWxBzmfNX75CKA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC299E?qs=j01uVdFEFjH9xb8%2Fvs53hw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC390E?qs=sGAEpiMZZMtOXy69nW9rM0%2FHbfl0f%252B3pZcjQYqVUphI%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/SN74HC573AN?qs=%252BWCn1GN4mVzruISjDLpAxw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/onsemi-Fairchild/1N914B?qs=sGAEpiMZZMtbRapU8LlZDzCgIkNleXIZjCSZIvAdjSc%3D</t>
+  </si>
+  <si>
+    <t>KingBright appears to have suitable LED's in 5mm, T-1 3/4 Lens Size</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/c/optoelectronics/led-lighting/led-emitters/standard-leds-through-hole/?m=Kingbright&amp;package%20%2F%20case=T-1%203%2F4%20%285%20mm%29</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECE-A1VKA100B?qs=sGAEpiMZZMsh%252B1woXyUXj%2FCjDN34kA%252BzNH8IV1070Pk%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/RCER71H104K0K1H03B?qs=Zt%252BKPUOg4of53jbypBpoRQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/C412C104K5R5TA7200?qs=mslOTO5mZ0hrfja2YJ2FJQ%3D%3D</t>
+  </si>
+  <si>
+    <t>1.0uf Electrolytic/Tantalum</t>
+  </si>
+  <si>
+    <t>1.0uf Electrolytic/Tantalum Radial</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/KEMET/T356A105M035AT?qs=r%2FVmNO8Tjq7kzg9AQX7h%2Fg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/kyocera-avx/TAP105K025SRW/1471039</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kyocera-avx/TAP105K025SRW/1471039</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/CF14JT4K70?qs=sGAEpiMZZMtlubZbdhIBIA%252B43obPAL0t3ls3NS%252BkwXU%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/CF14JT10K0?qs=FESYatJ8odJcEE4HXxUVCA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/CF14JT2K00?qs=sGAEpiMZZMtlubZbdhIBIA%252B43obPAL0tRPOdOjnFeEY%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/CF14JT1K00?qs=FESYatJ8odLLAkjsom%2FJYQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/RNMF14FTC22K0?qs=FESYatJ8odKP4NN%2F7NHPUQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Bourns/4609X-101-331LF?qs=9G919%252BqIayYLRuazsZszxw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Amphenol-FCI/68691-440HLF?qs=cPwqfQhQFYMYN3UF9G02MQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/ITT-Cannon/DE-9S-1A2N-A197?qs=5aG0NVq1C4yMlVT5f5i9rg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/STMicroelectronics/L78L33ABZ-AP?qs=7IaIRco65plqHZGvVBuyKw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/MAX232N?qs=5BZzbFV4k2vm92DEZa5XUA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD4051BE?qs=q2XTDbzbm6DxulBsMcV7tA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HC00E?qs=UGVLDq%2F29ujRl31yA9SdhQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74HC04N?qs=L5CvrNUdZirrSGYiJvTylA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74HC27N?qs=sGAEpiMZZMv4BkFy%252BbL2aPi%252BL8sNTlmrokzu%2FObU0qc%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HC30E?qs=tJ5HNKWh3OVq%2F4Pt68gHgg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HC32E?qs=tJ5HNKWh3OWln99ctEO0hw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74HC74N?qs=p6YqzpSxLIzMm7Vo1aTZ0w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HC157E?qs=YxwvVplHM%2Fl8uv0E9i2LyA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HC238E?qs=xFfolx0DHx2djOhmdGyl2g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74LS259BN?qs=SL3LIuy2dWxBzmfNX75CKA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HC299E?qs=j01uVdFEFjH9xb8%2Fvs53hw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HC390E?qs=sGAEpiMZZMtOXy69nW9rM0%2FHbfl0f%252B3pZcjQYqVUphI%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74HC573AN?qs=%252BWCn1GN4mVzruISjDLpAxw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/onsemi-Fairchild/1N914B?qs=sGAEpiMZZMtbRapU8LlZDzCgIkNleXIZjCSZIvAdjSc%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/c/optoelectronics/led-lighting/led-emitters/standard-leds-through-hole/?m=Kingbright&amp;package%20%2F%20case=T-1%203%2F4%20%285%20mm%29</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/ECE-A1VKA100B?qs=sGAEpiMZZMsh%252B1woXyUXj%2FCjDN34kA%252BzNH8IV1070Pk%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Murata-Electronics/RCER71H104K0K1H03B?qs=Zt%252BKPUOg4of53jbypBpoRQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/C412C104K5R5TA7200?qs=mslOTO5mZ0hrfja2YJ2FJQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/T356A105M035AT?qs=r%2FVmNO8Tjq7kzg9AQX7h%2Fg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CF14JT4K70?qs=sGAEpiMZZMtlubZbdhIBIA%252B43obPAL0t3ls3NS%252BkwXU%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CF14JT10K0?qs=FESYatJ8odJcEE4HXxUVCA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CF14JT2K00?qs=sGAEpiMZZMtlubZbdhIBIA%252B43obPAL0tRPOdOjnFeEY%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CF14JT1K00?qs=FESYatJ8odLLAkjsom%2FJYQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/RNMF14FTC22K0?qs=FESYatJ8odKP4NN%2F7NHPUQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/4609X-101-331LF?qs=9G919%252BqIayYLRuazsZszxw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Amphenol-FCI/68691-440HLF?qs=cPwqfQhQFYMYN3UF9G02MQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ITT-Cannon/DE-9S-1A2N-A197?qs=5aG0NVq1C4yMlVT5f5i9rg%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -982,7 +1267,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1006,7 +1291,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1363,46 +1647,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="73" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
     <col min="6" max="6" width="95.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1411,16 +1695,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1428,16 +1712,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1445,16 +1729,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1462,16 +1746,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3">
         <v>628128</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -1480,17 +1764,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12" t="s">
-        <v>142</v>
+        <v>128</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1498,16 +1781,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1515,16 +1798,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1532,16 +1815,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1549,16 +1832,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1566,16 +1849,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1583,16 +1866,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1600,16 +1883,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1617,16 +1900,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1634,16 +1917,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1651,16 +1934,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1668,16 +1951,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1685,21 +1968,21 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1707,21 +1990,21 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1729,24 +2012,24 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1757,13 +2040,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1771,16 +2054,16 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1788,16 +2071,16 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1805,21 +2088,21 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1827,16 +2110,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1844,16 +2127,16 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1861,16 +2144,16 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1878,16 +2161,16 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1895,16 +2178,16 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1912,21 +2195,21 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C35" s="3">
         <v>330</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1934,16 +2217,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" t="s">
         <v>10</v>
       </c>
-      <c r="D37" t="s">
-        <v>11</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1951,16 +2234,19 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1</v>
+        <v>129</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1968,33 +2254,36 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="D39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1</v>
+        <v>134</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2002,66 +2291,2217 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="3">
-        <v>5</v>
-      </c>
-      <c r="D41" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" t="s">
-        <v>1</v>
+        <v>124</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F12" r:id="rId2"/>
-    <hyperlink ref="F10" r:id="rId3"/>
-    <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F13" r:id="rId5"/>
-    <hyperlink ref="F16" r:id="rId6"/>
-    <hyperlink ref="F14" r:id="rId7"/>
-    <hyperlink ref="F4" r:id="rId8"/>
-    <hyperlink ref="F8" r:id="rId9"/>
-    <hyperlink ref="F18" r:id="rId10"/>
-    <hyperlink ref="F15" r:id="rId11"/>
-    <hyperlink ref="F17" r:id="rId12"/>
-    <hyperlink ref="F19" r:id="rId13"/>
-    <hyperlink ref="F11" r:id="rId14"/>
-    <hyperlink ref="F21" r:id="rId15"/>
-    <hyperlink ref="F23" r:id="rId16"/>
-    <hyperlink ref="F25" r:id="rId17"/>
-    <hyperlink ref="F26" r:id="rId18"/>
-    <hyperlink ref="F28" r:id="rId19"/>
-    <hyperlink ref="F27" r:id="rId20"/>
-    <hyperlink ref="F31" r:id="rId21"/>
-    <hyperlink ref="F32" r:id="rId22"/>
-    <hyperlink ref="F30" r:id="rId23"/>
-    <hyperlink ref="F33" r:id="rId24"/>
-    <hyperlink ref="F34" r:id="rId25"/>
-    <hyperlink ref="F35" r:id="rId26"/>
-    <hyperlink ref="F37" r:id="rId27"/>
-    <hyperlink ref="F7" r:id="rId28"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F23" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F27" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F31" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F32" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F30" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F34" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F35" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F7" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F38" r:id="rId29" xr:uid="{49D49006-C9F7-ED44-A76E-2946B81A6EFE}"/>
+    <hyperlink ref="F39" r:id="rId30" xr:uid="{A9AEA434-CEAD-1E42-8B4A-064744984108}"/>
+    <hyperlink ref="F40" r:id="rId31" xr:uid="{490AEF5A-4ECD-D740-8F00-33E8CD5B5A45}"/>
+    <hyperlink ref="F41" r:id="rId32" xr:uid="{211A208D-00B3-0641-BAD8-19118499D777}"/>
+    <hyperlink ref="F42" r:id="rId33" xr:uid="{4C29C955-5C8E-4348-B4AE-B984E37AC633}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47F7A7A-0D93-384D-B9EF-DFF4AEDEF130}">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="95.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3">
+        <v>628128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="3">
+        <v>330</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{745F7732-D253-454C-8835-259F9A3C1F53}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{B8C6E343-1A4A-E142-9135-3C4BE40A5E7A}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{384B3FF2-15B0-694B-95B0-BB3486F48F2F}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{A25D9E23-387E-1D4C-BD30-3FCDBBFD0B1C}"/>
+    <hyperlink ref="F13" r:id="rId5" xr:uid="{158AC3F1-0048-8743-A6A8-3107E97C8E55}"/>
+    <hyperlink ref="F16" r:id="rId6" xr:uid="{CCAAFA5A-708A-3143-899B-D15E54E3DBF4}"/>
+    <hyperlink ref="F14" r:id="rId7" xr:uid="{F9A1160E-9A4D-634A-AB23-05BFEFD861A6}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{3D388FA2-823B-D348-956D-F94035B8B6C0}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{6821180D-F62E-CC42-A349-8E7A3635AE3B}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{442C2F78-D180-DB46-93F0-3FE9A3FE60E3}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{3EDC4253-87A2-8941-960B-2FB720D13638}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{549D4658-9690-BF40-834F-017ED57313DF}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{1F4C462E-53D0-0F45-AE5D-B5DCE49996B4}"/>
+    <hyperlink ref="F11" r:id="rId14" xr:uid="{8B28F4C2-FE9A-1646-80AF-80911A52721D}"/>
+    <hyperlink ref="F21" r:id="rId15" xr:uid="{74997DAE-5A27-5F4B-8F32-98242BBFA84C}"/>
+    <hyperlink ref="F23" r:id="rId16" xr:uid="{45C1DAAA-0E80-7E4E-ABC7-E242BF576429}"/>
+    <hyperlink ref="F25" r:id="rId17" xr:uid="{5A48FB41-8EC4-F244-B750-DEDD15C4977B}"/>
+    <hyperlink ref="F26" r:id="rId18" xr:uid="{F6F55993-47BA-9B4B-9736-3BC75B193BC2}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{07DEAED9-EF2F-2E4F-8E32-A6E22E8080FE}"/>
+    <hyperlink ref="F27" r:id="rId20" xr:uid="{07CA6727-AA92-9F41-8833-A1EC10D64844}"/>
+    <hyperlink ref="F31" r:id="rId21" xr:uid="{51D27CAE-BD0C-6448-BE38-DB1D3AD81196}"/>
+    <hyperlink ref="F32" r:id="rId22" xr:uid="{65D547FB-2306-AC4A-B3DA-CA3555A48742}"/>
+    <hyperlink ref="F30" r:id="rId23" xr:uid="{12526484-304D-C34A-A39C-9C2A66CA584B}"/>
+    <hyperlink ref="F33" r:id="rId24" xr:uid="{70F67950-8EAF-324F-AD7E-24BFC2E4A70D}"/>
+    <hyperlink ref="F34" r:id="rId25" xr:uid="{992DF2CD-AB4C-2C4F-B934-B53F9E082D54}"/>
+    <hyperlink ref="F35" r:id="rId26" xr:uid="{2E2CC33D-6D7F-2B47-942D-47EFF11D8118}"/>
+    <hyperlink ref="F37" r:id="rId27" xr:uid="{3DF8C1A4-328D-C34D-A56C-6E646E560D90}"/>
+    <hyperlink ref="F7" r:id="rId28" xr:uid="{45EE5D7C-040F-2B45-8AF1-ED45005E43B1}"/>
+    <hyperlink ref="F38" r:id="rId29" xr:uid="{CBAC0EDC-0A4B-4F4E-8B14-32C9D6F84670}"/>
+    <hyperlink ref="F39" r:id="rId30" xr:uid="{FE22DD71-BC57-BF4E-8EC5-9EB95CB9023A}"/>
+    <hyperlink ref="F40" r:id="rId31" xr:uid="{E4C0D3A1-E1ED-6B44-84C0-6A6F3F6C2642}"/>
+    <hyperlink ref="F41" r:id="rId32" xr:uid="{02D45E3F-76C3-814F-86D9-F3417A49192E}"/>
+    <hyperlink ref="F42" r:id="rId33" xr:uid="{FB1EADA9-6D27-694D-A8E1-5968FDC76086}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69139381-9CC4-E949-991F-4D66AD9220B5}">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="95.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3">
+        <v>628128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="3">
+        <v>330</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{721E78E2-26E1-FB40-B515-A9274EFBA44D}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{22A4C150-9996-BF44-87E4-06BC17C552D1}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{0C5F7E7D-5ADE-744D-9A40-1FA9D5933849}"/>
+    <hyperlink ref="F10" r:id="rId4" xr:uid="{140C4106-8731-104B-A96E-E2B76E0A9B18}"/>
+    <hyperlink ref="F11" r:id="rId5" xr:uid="{8FF2612F-178D-364A-880A-62B9F48ABFA0}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{C100ACAD-E581-C64A-9E4F-AC822D58019B}"/>
+    <hyperlink ref="F13" r:id="rId7" xr:uid="{F87AED2C-8496-E14E-A7C3-6794406FE306}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{1BBCDDC9-DF7B-9649-8BBC-46E9875051A7}"/>
+    <hyperlink ref="F15" r:id="rId9" xr:uid="{8815F82A-7758-034A-B802-7028E2DD283A}"/>
+    <hyperlink ref="F16" r:id="rId10" xr:uid="{4ED352F7-1526-9C46-B011-46FF0D64D5B6}"/>
+    <hyperlink ref="F17" r:id="rId11" xr:uid="{48D6AA81-A185-B340-AC85-CAE7CED208E0}"/>
+    <hyperlink ref="F18" r:id="rId12" xr:uid="{17214D72-91D2-3641-B983-5C14382B6251}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{532BEEFA-272F-AB4C-9243-4D1D757CDE03}"/>
+    <hyperlink ref="F21" r:id="rId14" xr:uid="{D689AC4D-5954-6241-A355-FD117CE4891C}"/>
+    <hyperlink ref="F23" r:id="rId15" xr:uid="{71E7480E-DFAF-E644-B5F4-1FC17788CBC9}"/>
+    <hyperlink ref="F25" r:id="rId16" xr:uid="{4ED61E6A-56C7-E244-9EEF-14113CD6D907}"/>
+    <hyperlink ref="F26" r:id="rId17" xr:uid="{CD91F830-3F8F-4349-A603-8E7651C1B034}"/>
+    <hyperlink ref="F27" r:id="rId18" xr:uid="{1E1DCCAA-DBEF-E44D-9ED8-B9DCAEE4B256}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{54E3ED3B-77A5-CE49-972B-0C5359F565C1}"/>
+    <hyperlink ref="F30" r:id="rId20" xr:uid="{62675F50-D6EE-1444-B43C-E541F96F5E66}"/>
+    <hyperlink ref="F31" r:id="rId21" xr:uid="{207F56DA-2381-D84A-98B8-B2B4D3E08C0A}"/>
+    <hyperlink ref="F32" r:id="rId22" xr:uid="{221E802A-A8A9-3243-9AD5-D72EB29B4D4D}"/>
+    <hyperlink ref="F38" r:id="rId23" xr:uid="{5ABECF2C-1D20-6B43-A561-35F1E6A5DF09}"/>
+    <hyperlink ref="F42" r:id="rId24" xr:uid="{211B71BA-5DEB-A64A-80A9-FEB7DC067D30}"/>
+    <hyperlink ref="F37" r:id="rId25" xr:uid="{7961E239-D8BA-1E40-80F2-23F0BE943A1D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626A541B-A088-EE47-8090-9C2E4675A8E6}">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="95.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3">
+        <v>628128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="3">
+        <v>330</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{48ED59AB-1577-5744-BBE5-2D0CFD741881}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{0B817C48-5AD0-4B44-9D87-3D2B55DB0B4A}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{A1FD087D-A790-EE4B-A095-70ED10D1E47B}"/>
+    <hyperlink ref="F10" r:id="rId4" xr:uid="{EE53B8E7-4BB3-A34D-9A86-E751A6B31B73}"/>
+    <hyperlink ref="F11" r:id="rId5" xr:uid="{7325341D-8B9A-0B4A-AB51-95EC2C445E22}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{5E519349-BCB0-BB45-8872-7C84EDA7B610}"/>
+    <hyperlink ref="F13" r:id="rId7" xr:uid="{05EDC8DD-C497-1243-B7E8-BBE2FC394DFB}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{03EBF04B-26FF-C94B-970E-3980000F190C}"/>
+    <hyperlink ref="F15" r:id="rId9" xr:uid="{D288304F-C620-3A4B-B64D-9B3621EB3321}"/>
+    <hyperlink ref="F16" r:id="rId10" xr:uid="{DB8757E9-C9BF-DB46-AD1B-545CFBADE15A}"/>
+    <hyperlink ref="F17" r:id="rId11" xr:uid="{307BA185-DE15-154C-AE4C-9F34D5D6A88B}"/>
+    <hyperlink ref="F18" r:id="rId12" xr:uid="{3D5271D1-32BB-774D-BC07-63DDFAFBD1C7}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{B8431060-2EAD-1E4A-A683-296BEDEEDA66}"/>
+    <hyperlink ref="F21" r:id="rId14" xr:uid="{4FEA0D87-9274-5342-A3FE-A8C9AC6392B8}"/>
+    <hyperlink ref="F23" r:id="rId15" xr:uid="{FACC0215-8FAB-7543-A0E1-18C7A2E17F66}"/>
+    <hyperlink ref="F25" r:id="rId16" xr:uid="{FCC8B924-BB43-7241-914B-6761C3CB1877}"/>
+    <hyperlink ref="F26" r:id="rId17" xr:uid="{D8B9D0B4-E1EF-294F-9495-2D5E387044DB}"/>
+    <hyperlink ref="F27" r:id="rId18" xr:uid="{97395ED2-066B-094F-9F48-2AE47E1293F3}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{1EF9CC13-2791-174D-87F8-551838329AAF}"/>
+    <hyperlink ref="F30" r:id="rId20" xr:uid="{EB0503CF-6262-744E-A8CC-E8C65D4160DF}"/>
+    <hyperlink ref="F31" r:id="rId21" xr:uid="{DF303D02-AD35-B643-937C-F9350CAD5DAB}"/>
+    <hyperlink ref="F32" r:id="rId22" xr:uid="{E6E9C25D-4BC3-D246-897B-41B8D140C621}"/>
+    <hyperlink ref="F38" r:id="rId23" xr:uid="{C4AD5DD3-087E-1841-AC77-193FE320B46A}"/>
+    <hyperlink ref="F42" r:id="rId24" xr:uid="{25556FB5-C112-FD47-B3AD-A6E5595B3BFF}"/>
+    <hyperlink ref="F37" r:id="rId25" xr:uid="{B11BDC03-C1A2-F74E-87FA-6793532E7038}"/>
+    <hyperlink ref="F3" r:id="rId26" xr:uid="{A9DFE75E-89EA-E646-9A23-D1D33FA18040}"/>
+    <hyperlink ref="F4" r:id="rId27" xr:uid="{034B8516-2976-A24D-8481-6DE1C60633D9}"/>
+    <hyperlink ref="F33" r:id="rId28" xr:uid="{0835D557-85D2-9847-AC48-99C1B73250BE}"/>
+    <hyperlink ref="F34" r:id="rId29" xr:uid="{5E4B7CDA-3E66-1848-9914-25B6D6CC6890}"/>
+    <hyperlink ref="F35" r:id="rId30" xr:uid="{B81E2C39-9B37-1344-96E4-7CDC349A896D}"/>
+    <hyperlink ref="F39" r:id="rId31" xr:uid="{DDC137CE-4D91-1042-8613-268D45711AC4}"/>
+    <hyperlink ref="F40" r:id="rId32" xr:uid="{1CB8AD5A-AF0A-3D4F-804D-2BA0B07EC37B}"/>
+    <hyperlink ref="F41" r:id="rId33" xr:uid="{92655E09-1745-4A4F-B068-9466560552F7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>